<commit_message>
ep02 day1,2 대사 엑셀 수정.
-대사 수정 및 양식 변경 적용
-2D애니메이션 폴더 정리 및 위치 변경
</commit_message>
<xml_diff>
--- a/Excel2Json/bin/ep02/ep02_1.xlsx
+++ b/Excel2Json/bin/ep02/ep02_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justb\Documents\GitHub\Slanted_Structure\Excel2Json\bin\ep02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0F53FB-6613-42E5-9065-5F85787CFC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB17131E-AC22-4ED6-B9C5-5214E051B264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="201010" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="201110_speat" sheetId="31" r:id="rId6"/>
     <sheet name="201120" sheetId="29" r:id="rId7"/>
     <sheet name="201130" sheetId="30" r:id="rId8"/>
+    <sheet name="202010" sheetId="32" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -312,8 +313,42 @@
 </comments>
 </file>
 
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>훠이</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{876D6060-652B-468E-92CA-DBA927B2BEBD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>0: Idle
+1: Laugh
+2: Sad
+3: Cry
+4: Angry
+5: Surprise
+6: Panic
+7: Suspicion
+8: Fear
+9: Curious</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="134">
   <si>
     <t>이름</t>
   </si>
@@ -321,9 +356,6 @@
     <t>표정</t>
   </si>
   <si>
-    <t>종류</t>
-  </si>
-  <si>
     <t>내용</t>
   </si>
   <si>
@@ -336,15 +368,9 @@
     <t>expression</t>
   </si>
   <si>
-    <t>kind</t>
-  </si>
-  <si>
     <t>contents</t>
   </si>
   <si>
-    <t>Main Char</t>
-  </si>
-  <si>
     <t>라우</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -353,14 +379,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Main Char</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>201010</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -743,6 +761,38 @@
   </si>
   <si>
     <t>201110_speat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애니메이터 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>anim_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rhina</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rau</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>202010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어제랑 다른 곳으로 한번 가봐야 겠다!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1137,25 +1187,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5A58F5-DB17-4210-ACBF-521534671DF7}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="27.375" customWidth="1"/>
-    <col min="4" max="4" width="47.75" customWidth="1"/>
+    <col min="2" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="27.375" customWidth="1"/>
+    <col min="5" max="5" width="47.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1163,130 +1213,128 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1298,25 +1346,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD3D267-149A-4874-91EC-FEEC24D1F08D}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="63.625" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="2" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="63.625" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1324,102 +1372,99 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="33">
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="33">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="4"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="1"/>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1431,25 +1476,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{039EFBE4-104A-486E-865E-1F2F8786AE25}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="63.625" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="2" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="63.625" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1457,83 +1502,83 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="4"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="1"/>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1545,25 +1590,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3005710-42CA-4ECD-A056-329BD01613B7}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="63.625" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="2" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="63.625" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1571,138 +1616,129 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1717,19 +1753,19 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="63.625" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="2" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="63.625" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1740,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -1748,104 +1784,104 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
+      <c r="C8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
+      <c r="C9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1859,20 +1895,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEB8412-65D6-4165-B40B-CFF950032322}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="63.625" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="2" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="63.625" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1883,7 +1919,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -1891,296 +1927,296 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" t="s">
         <v>37</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2193,23 +2229,25 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC786CA-1FCC-41E7-8EBE-7AA7CB117CFF}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="63.625" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="2" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="63.625" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2217,94 +2255,94 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="4"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2318,21 +2356,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2B45FD-C5C1-47EC-ACF8-B88135AF9AC4}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="63.625" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="63.625" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>129</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
@@ -2342,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -2350,935 +2390,1083 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>9</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
+      <c r="C8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
+      <c r="C9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
+      <c r="C10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>130</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15" t="s">
-        <v>71</v>
-      </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B22">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B38">
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="D48" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="D52" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="D54" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="D55" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="B59">
         <v>0</v>
       </c>
-      <c r="C59" t="s">
-        <v>114</v>
-      </c>
       <c r="D59" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D61" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="C63" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="D64" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B65">
         <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D65" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D67" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B68">
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>131</v>
+      </c>
+      <c r="D69" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84443E4E-291D-4A68-93F5-2EB598A7EA41}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="27.375" customWidth="1"/>
+    <col min="5" max="5" width="47.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B69">
-        <v>0</v>
-      </c>
-      <c r="C69" t="s">
-        <v>124</v>
-      </c>
-      <c r="D69" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>